<commit_message>
entity has changed update
</commit_message>
<xml_diff>
--- a/upload_files/CV2__JL1_-_Oracle.xlsx
+++ b/upload_files/CV2__JL1_-_Oracle.xlsx
@@ -502,61 +502,61 @@
     <t>pl/sql : 2</t>
   </si>
   <si>
+    <t>administration : 2</t>
+  </si>
+  <si>
+    <t>oracle rac : 2</t>
+  </si>
+  <si>
+    <t>database : 1</t>
+  </si>
+  <si>
+    <t>oracle : 11</t>
+  </si>
+  <si>
+    <t>enterprise manager : 1</t>
+  </si>
+  <si>
+    <t>production : 1</t>
+  </si>
+  <si>
+    <t>linux : 1</t>
+  </si>
+  <si>
     <t>rac : 1</t>
   </si>
   <si>
-    <t>linux : 1</t>
-  </si>
-  <si>
-    <t>database : 1</t>
-  </si>
-  <si>
-    <t>oracle rac : 2</t>
-  </si>
-  <si>
-    <t>production : 1</t>
+    <t>rman : 1</t>
   </si>
   <si>
     <t>manager : 1</t>
   </si>
   <si>
-    <t>administration : 2</t>
-  </si>
-  <si>
-    <t>rman : 1</t>
-  </si>
-  <si>
-    <t>enterprise manager : 1</t>
-  </si>
-  <si>
-    <t>oracle : 11</t>
-  </si>
-  <si>
     <t>90.90</t>
   </si>
   <si>
     <t>communication skills : 2</t>
   </si>
   <si>
+    <t>linux : 2</t>
+  </si>
+  <si>
+    <t>red hat : 2</t>
+  </si>
+  <si>
+    <t>management : 1</t>
+  </si>
+  <si>
+    <t>process : 1</t>
+  </si>
+  <si>
+    <t>design : 1</t>
+  </si>
+  <si>
     <t>tools : 1</t>
   </si>
   <si>
-    <t>linux : 2</t>
-  </si>
-  <si>
-    <t>management : 1</t>
-  </si>
-  <si>
-    <t>red hat : 2</t>
-  </si>
-  <si>
     <t>scripting : 1</t>
-  </si>
-  <si>
-    <t>design : 1</t>
-  </si>
-  <si>
-    <t>process : 1</t>
   </si>
   <si>
     <t>42.85</t>

</xml_diff>